<commit_message>
Fix campaign names, id dup email addresses, add gift type and cat
- Fix campaign names for all input files instead of just QB
- Identify email addresses/names that match more than one account
- Add Gift Type and Gift Category columns to all output
</commit_message>
<xml_diff>
--- a/donor_update/sample_files/qb.xlsx
+++ b/donor_update/sample_files/qb.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>December 24, 2021 - February 15, 2022</t>
+  </si>
+  <si>
+    <t>Our Forever Home</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ _€"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -156,6 +159,12 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -209,6 +218,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,7 +528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,7 +539,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,8 +670,8 @@
         <v>14</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>13</v>
+      <c r="G9" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="4">
@@ -897,5 +909,6 @@
     <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>